<commit_message>
Edit Linear Regression data for tech Industries and Add Logistic Regression in R file
</commit_message>
<xml_diff>
--- a/R/x_raw_y_tech_excel.xlsx
+++ b/R/x_raw_y_tech_excel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>SP500</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -947,7 +944,7 @@
   <dimension ref="A1:R203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12333,8 +12330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R206"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12404,7 +12401,7 @@
         <v>36738</v>
       </c>
       <c r="B2">
-        <v>-6.3611388000000005E-2</v>
+        <v>120.2813</v>
       </c>
       <c r="C2">
         <v>10357.445</v>
@@ -12451,8 +12448,8 @@
       <c r="Q2">
         <v>6.36</v>
       </c>
-      <c r="R2" t="s">
-        <v>21</v>
+      <c r="R2">
+        <v>1430.83</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -12460,7 +12457,7 @@
         <v>36769</v>
       </c>
       <c r="B3">
-        <v>-0.11843137300000001</v>
+        <v>136.8125</v>
       </c>
       <c r="C3">
         <v>10357.445</v>
@@ -12508,7 +12505,7 @@
         <v>6.45</v>
       </c>
       <c r="R3">
-        <v>6.069903482594019E-2</v>
+        <v>1517.68</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -12516,7 +12513,7 @@
         <v>36799</v>
       </c>
       <c r="B4">
-        <v>-8.3723127999999994E-2</v>
+        <v>116.0625</v>
       </c>
       <c r="C4">
         <v>10357.445</v>
@@ -12564,7 +12561,7 @@
         <v>7.29</v>
       </c>
       <c r="R4">
-        <v>-5.3482947656950164E-2</v>
+        <v>1436.51</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
@@ -12572,7 +12569,7 @@
         <v>36830</v>
       </c>
       <c r="B5">
-        <v>4.9001100999999998E-2</v>
+        <v>106.6875</v>
       </c>
       <c r="C5">
         <v>10472.285</v>
@@ -12620,7 +12617,7 @@
         <v>8.09</v>
       </c>
       <c r="R5">
-        <v>-4.9494956526581202E-3</v>
+        <v>1429.4</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -12628,7 +12625,7 @@
         <v>36860</v>
       </c>
       <c r="B6">
-        <v>7.5443199999999998E-4</v>
+        <v>81.6875</v>
       </c>
       <c r="C6">
         <v>10472.285</v>
@@ -12676,7 +12673,7 @@
         <v>9.01</v>
       </c>
       <c r="R6">
-        <v>-8.0068560235063702E-2</v>
+        <v>1314.95</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
@@ -12684,7 +12681,7 @@
         <v>36891</v>
       </c>
       <c r="B7">
-        <v>-6.6877822000000003E-2</v>
+        <v>74.5625</v>
       </c>
       <c r="C7">
         <v>10472.285</v>
@@ -12732,7 +12729,7 @@
         <v>8.4600000000000009</v>
       </c>
       <c r="R7">
-        <v>4.0533860603064742E-3</v>
+        <v>1320.28</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
@@ -12740,7 +12737,7 @@
         <v>36922</v>
       </c>
       <c r="B8">
-        <v>0.10976625</v>
+        <v>87.4</v>
       </c>
       <c r="C8">
         <v>10508.120999999999</v>
@@ -12788,7 +12785,7 @@
         <v>7.61</v>
       </c>
       <c r="R8">
-        <v>3.4636592238010078E-2</v>
+        <v>1366.01</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
@@ -12796,7 +12793,7 @@
         <v>36950</v>
       </c>
       <c r="B9">
-        <v>-2.3199022999999999E-2</v>
+        <v>62</v>
       </c>
       <c r="C9">
         <v>10508.120999999999</v>
@@ -12844,7 +12841,7 @@
         <v>7.92</v>
       </c>
       <c r="R9">
-        <v>-9.2290686012547418E-2</v>
+        <v>1239.94</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -12852,7 +12849,7 @@
         <v>36981</v>
       </c>
       <c r="B10">
-        <v>3.9225299999999996E-3</v>
+        <v>53.3</v>
       </c>
       <c r="C10">
         <v>10508.120999999999</v>
@@ -12900,7 +12897,7 @@
         <v>8.5</v>
       </c>
       <c r="R10">
-        <v>-6.4204719583205727E-2</v>
+        <v>1160.33</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
@@ -12908,7 +12905,7 @@
         <v>37011</v>
       </c>
       <c r="B11">
-        <v>-5.1174692000000001E-2</v>
+        <v>63.7</v>
       </c>
       <c r="C11">
         <v>10638.384</v>
@@ -12956,7 +12953,7 @@
         <v>7.69</v>
       </c>
       <c r="R11">
-        <v>7.6814354537071416E-2</v>
+        <v>1249.46</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
@@ -12964,7 +12961,7 @@
         <v>37042</v>
       </c>
       <c r="B12">
-        <v>1.8720378999999999E-2</v>
+        <v>60.4</v>
       </c>
       <c r="C12">
         <v>10638.384</v>
@@ -13012,7 +13009,7 @@
         <v>8.06</v>
       </c>
       <c r="R12">
-        <v>5.0901989659533076E-3</v>
+        <v>1255.82</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
@@ -13020,7 +13017,7 @@
         <v>37072</v>
       </c>
       <c r="B13">
-        <v>7.9145888999999997E-2</v>
+        <v>61.5</v>
       </c>
       <c r="C13">
         <v>10638.384</v>
@@ -13068,7 +13065,7 @@
         <v>8.26</v>
       </c>
       <c r="R13">
-        <v>-2.5003583316080213E-2</v>
+        <v>1224.42</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
@@ -13076,7 +13073,7 @@
         <v>37103</v>
       </c>
       <c r="B14">
-        <v>4.8110425999999998E-2</v>
+        <v>57</v>
       </c>
       <c r="C14">
         <v>10639.486000000001</v>
@@ -13124,7 +13121,7 @@
         <v>8.0500000000000007</v>
       </c>
       <c r="R14">
-        <v>-1.0772447362833004E-2</v>
+        <v>1211.23</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
@@ -13132,7 +13129,7 @@
         <v>37134</v>
       </c>
       <c r="B15">
-        <v>1.5790907E-2</v>
+        <v>49.5</v>
       </c>
       <c r="C15">
         <v>10639.486000000001</v>
@@ -13180,7 +13177,7 @@
         <v>9.24</v>
       </c>
       <c r="R15">
-        <v>-6.4108385690579084E-2</v>
+        <v>1133.58</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
@@ -13188,7 +13185,7 @@
         <v>37164</v>
       </c>
       <c r="B16">
-        <v>0.106325301</v>
+        <v>38.65</v>
       </c>
       <c r="C16">
         <v>10639.486000000001</v>
@@ -13236,7 +13233,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="R16">
-        <v>-8.1723389615201314E-2</v>
+        <v>1040.94</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
@@ -13244,7 +13241,7 @@
         <v>37195</v>
       </c>
       <c r="B17">
-        <v>3.5074044999999998E-2</v>
+        <v>47</v>
       </c>
       <c r="C17">
         <v>10701.316999999999</v>
@@ -13292,7 +13289,7 @@
         <v>8.7899999999999991</v>
       </c>
       <c r="R17">
-        <v>1.8099025880454089E-2</v>
+        <v>1059.78</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
@@ -13300,7 +13297,7 @@
         <v>37225</v>
       </c>
       <c r="B18">
-        <v>3.7019074999999999E-2</v>
+        <v>54</v>
       </c>
       <c r="C18">
         <v>10701.316999999999</v>
@@ -13348,7 +13345,7 @@
         <v>8.2899999999999991</v>
       </c>
       <c r="R18">
-        <v>7.5175979920360847E-2</v>
+        <v>1139.45</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
@@ -13356,7 +13353,7 @@
         <v>37256</v>
       </c>
       <c r="B19">
-        <v>-3.2984210999999999E-2</v>
+        <v>53.2</v>
       </c>
       <c r="C19">
         <v>10701.316999999999</v>
@@ -13404,7 +13401,7 @@
         <v>8.15</v>
       </c>
       <c r="R19">
-        <v>7.5738294791345417E-3</v>
+        <v>1148.08</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
@@ -13412,7 +13409,7 @@
         <v>37287</v>
       </c>
       <c r="B20">
-        <v>4.1008950000000002E-2</v>
+        <v>53.7</v>
       </c>
       <c r="C20">
         <v>10834.445</v>
@@ -13460,7 +13457,7 @@
         <v>8.1</v>
       </c>
       <c r="R20">
-        <v>-1.5573827607832103E-2</v>
+        <v>1130.2</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
@@ -13468,7 +13465,7 @@
         <v>37315</v>
       </c>
       <c r="B21">
-        <v>1.1522634E-2</v>
+        <v>45.9</v>
       </c>
       <c r="C21">
         <v>10834.445</v>
@@ -13516,7 +13513,7 @@
         <v>7.33</v>
       </c>
       <c r="R21">
-        <v>-2.0766236064413413E-2</v>
+        <v>1106.73</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
@@ -13524,7 +13521,7 @@
         <v>37346</v>
       </c>
       <c r="B22">
-        <v>-8.3018867999999996E-2</v>
+        <v>49.55</v>
       </c>
       <c r="C22">
         <v>10834.445</v>
@@ -13572,7 +13569,7 @@
         <v>7.16</v>
       </c>
       <c r="R22">
-        <v>3.6738861330225081E-2</v>
+        <v>1147.3900000000001</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
@@ -13580,7 +13577,7 @@
         <v>37376</v>
       </c>
       <c r="B23">
-        <v>1.0678871E-2</v>
+        <v>43.45</v>
       </c>
       <c r="C23">
         <v>10934.752</v>
@@ -13628,7 +13625,7 @@
         <v>7.03</v>
       </c>
       <c r="R23">
-        <v>-6.1417652236815723E-2</v>
+        <v>1076.92</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
@@ -13636,7 +13633,7 @@
         <v>37407</v>
       </c>
       <c r="B24">
-        <v>4.9639712000000003E-2</v>
+        <v>41.76</v>
       </c>
       <c r="C24">
         <v>10934.752</v>
@@ -13684,7 +13681,7 @@
         <v>7.98</v>
       </c>
       <c r="R24">
-        <v>-9.0814545184414452E-3</v>
+        <v>1067.1400000000001</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
@@ -13692,7 +13689,7 @@
         <v>37437</v>
       </c>
       <c r="B25">
-        <v>5.9731884999999998E-2</v>
+        <v>36.049999999999997</v>
       </c>
       <c r="C25">
         <v>10934.752</v>
@@ -13740,7 +13737,7 @@
         <v>9.36</v>
       </c>
       <c r="R25">
-        <v>-7.2464718781041104E-2</v>
+        <v>989.81</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
@@ -13748,7 +13745,7 @@
         <v>37468</v>
       </c>
       <c r="B26">
-        <v>0.150302557</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="C26">
         <v>11037.057000000001</v>
@@ -13796,7 +13793,7 @@
         <v>9.7899999999999991</v>
       </c>
       <c r="R26">
-        <v>-7.8994958628423539E-2</v>
+        <v>911.62</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
@@ -13804,7 +13801,7 @@
         <v>37499</v>
       </c>
       <c r="B27">
-        <v>-3.8656408000000003E-2</v>
+        <v>32.53</v>
       </c>
       <c r="C27">
         <v>11037.057000000001</v>
@@ -13852,7 +13849,7 @@
         <v>9.85</v>
       </c>
       <c r="R27">
-        <v>4.8814198898663452E-3</v>
+        <v>916.07</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
@@ -13860,7 +13857,7 @@
         <v>37529</v>
       </c>
       <c r="B28">
-        <v>0.15421269200000001</v>
+        <v>26.6</v>
       </c>
       <c r="C28">
         <v>11037.057000000001</v>
@@ -13908,7 +13905,7 @@
         <v>10.68</v>
       </c>
       <c r="R28">
-        <v>-0.11002434311788412</v>
+        <v>815.28</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.35">
@@ -13916,7 +13913,7 @@
         <v>37560</v>
       </c>
       <c r="B29">
-        <v>-6.4935100000000005E-4</v>
+        <v>32.25</v>
       </c>
       <c r="C29">
         <v>11103.834000000001</v>
@@ -13964,7 +13961,7 @@
         <v>9.65</v>
       </c>
       <c r="R29">
-        <v>8.644882739672255E-2</v>
+        <v>885.76</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
@@ -13972,7 +13969,7 @@
         <v>37590</v>
       </c>
       <c r="B30">
-        <v>-1.0706637999999999E-2</v>
+        <v>38.08</v>
       </c>
       <c r="C30">
         <v>11103.834000000001</v>
@@ -14020,7 +14017,7 @@
         <v>8.9600000000000009</v>
       </c>
       <c r="R30">
-        <v>5.7069635115606809E-2</v>
+        <v>936.31</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
@@ -14028,7 +14025,7 @@
         <v>37621</v>
       </c>
       <c r="B31">
-        <v>-2.4644946000000001E-2</v>
+        <v>32.5</v>
       </c>
       <c r="C31">
         <v>11103.834000000001</v>
@@ -14076,7 +14073,7 @@
         <v>8.18</v>
       </c>
       <c r="R31">
-        <v>-6.0332582157618608E-2</v>
+        <v>879.82</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
@@ -14084,7 +14081,7 @@
         <v>37652</v>
       </c>
       <c r="B32">
-        <v>3.3455644E-2</v>
+        <v>32.14</v>
       </c>
       <c r="C32">
         <v>11230.078</v>
@@ -14132,7 +14129,7 @@
         <v>8.43</v>
       </c>
       <c r="R32">
-        <v>-2.7414698461048825E-2</v>
+        <v>855.7</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
@@ -14140,7 +14137,7 @@
         <v>37680</v>
       </c>
       <c r="B33">
-        <v>4.9614862000000003E-2</v>
+        <v>32.56</v>
       </c>
       <c r="C33">
         <v>11230.078</v>
@@ -14188,7 +14185,7 @@
         <v>8.0399999999999991</v>
       </c>
       <c r="R33">
-        <v>-1.7003622764987791E-2</v>
+        <v>841.15</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
@@ -14196,7 +14193,7 @@
         <v>37711</v>
       </c>
       <c r="B34">
-        <v>-3.4769297999999997E-2</v>
+        <v>32.49</v>
       </c>
       <c r="C34">
         <v>11230.078</v>
@@ -14244,7 +14241,7 @@
         <v>7.02</v>
       </c>
       <c r="R34">
-        <v>8.3576056589194092E-3</v>
+        <v>848.18</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
@@ -14252,7 +14249,7 @@
         <v>37741</v>
       </c>
       <c r="B35">
-        <v>-6.7115463E-2</v>
+        <v>35.26</v>
       </c>
       <c r="C35">
         <v>11370.653</v>
@@ -14300,7 +14297,7 @@
         <v>6.64</v>
       </c>
       <c r="R35">
-        <v>8.1044117993822162E-2</v>
+        <v>916.92</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
@@ -14308,7 +14305,7 @@
         <v>37772</v>
       </c>
       <c r="B36">
-        <v>-9.4736842000000002E-2</v>
+        <v>38.89</v>
       </c>
       <c r="C36">
         <v>11370.653</v>
@@ -14356,7 +14353,7 @@
         <v>6.34</v>
       </c>
       <c r="R36">
-        <v>5.0898660733760925E-2</v>
+        <v>963.59</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.35">
@@ -14364,7 +14361,7 @@
         <v>37802</v>
       </c>
       <c r="B37">
-        <v>-9.2250899999999996E-4</v>
+        <v>38.61</v>
       </c>
       <c r="C37">
         <v>11370.653</v>
@@ -14412,7 +14409,7 @@
         <v>5.86</v>
       </c>
       <c r="R37">
-        <v>1.1322242862628284E-2</v>
+        <v>974.5</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.35">
@@ -14420,7 +14417,7 @@
         <v>37833</v>
       </c>
       <c r="B38">
-        <v>5.6942277999999999E-2</v>
+        <v>40.85</v>
       </c>
       <c r="C38">
         <v>11625.137000000001</v>
@@ -14468,7 +14465,7 @@
         <v>5.82</v>
       </c>
       <c r="R38">
-        <v>1.6223704463827593E-2</v>
+        <v>990.31</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.35">
@@ -14476,7 +14473,7 @@
         <v>37864</v>
       </c>
       <c r="B39">
-        <v>-5.044626E-3</v>
+        <v>43.49</v>
       </c>
       <c r="C39">
         <v>11625.137000000001</v>
@@ -14524,7 +14521,7 @@
         <v>5.36</v>
       </c>
       <c r="R39">
-        <v>1.7873191222950391E-2</v>
+        <v>1008.01</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.35">
@@ -14532,7 +14529,7 @@
         <v>37894</v>
       </c>
       <c r="B40">
-        <v>-3.8612199E-2</v>
+        <v>43.13</v>
       </c>
       <c r="C40">
         <v>11625.137000000001</v>
@@ -14580,7 +14577,7 @@
         <v>4.92</v>
       </c>
       <c r="R40">
-        <v>-1.1944325949147294E-2</v>
+        <v>995.97</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.35">
@@ -14588,7 +14585,7 @@
         <v>37925</v>
       </c>
       <c r="B41">
-        <v>-1.3978297000000001E-2</v>
+        <v>47.3</v>
       </c>
       <c r="C41">
         <v>11816.826999999999</v>
@@ -14636,7 +14633,7 @@
         <v>4.62</v>
       </c>
       <c r="R41">
-        <v>5.4961494824141255E-2</v>
+        <v>1050.71</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.35">
@@ -14644,7 +14641,7 @@
         <v>37955</v>
       </c>
       <c r="B42">
-        <v>-5.1235129999999997E-3</v>
+        <v>48.08</v>
       </c>
       <c r="C42">
         <v>11816.826999999999</v>
@@ -14692,7 +14689,7 @@
         <v>4.28</v>
       </c>
       <c r="R42">
-        <v>7.1285131006653124E-3</v>
+        <v>1058.2</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.35">
@@ -14700,7 +14697,7 @@
         <v>37986</v>
       </c>
       <c r="B43">
-        <v>-5.1050529999999997E-2</v>
+        <v>48.51</v>
       </c>
       <c r="C43">
         <v>11816.826999999999</v>
@@ -14748,7 +14745,7 @@
         <v>3.94</v>
       </c>
       <c r="R43">
-        <v>5.0765450765450693E-2</v>
+        <v>1111.92</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.35">
@@ -14756,7 +14753,7 @@
         <v>38017</v>
       </c>
       <c r="B44">
-        <v>-1.8073315999999999E-2</v>
+        <v>50.5</v>
       </c>
       <c r="C44">
         <v>11988.403</v>
@@ -14804,7 +14801,7 @@
         <v>4.26</v>
       </c>
       <c r="R44">
-        <v>1.7276422764227695E-2</v>
+        <v>1131.1300000000001</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.35">
@@ -14812,7 +14809,7 @@
         <v>38046</v>
       </c>
       <c r="B45">
-        <v>-1.8245732000000001E-2</v>
+        <v>48.94</v>
       </c>
       <c r="C45">
         <v>11988.403</v>
@@ -14860,7 +14857,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="R45">
-        <v>1.2209029908144986E-2</v>
+        <v>1144.94</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.35">
@@ -14868,7 +14865,7 @@
         <v>38077</v>
       </c>
       <c r="B46">
-        <v>-3.6691129999999999E-3</v>
+        <v>47.45</v>
       </c>
       <c r="C46">
         <v>11988.403</v>
@@ -14916,7 +14913,7 @@
         <v>3.98</v>
       </c>
       <c r="R46">
-        <v>-1.6358935839432598E-2</v>
+        <v>1126.21</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.35">
@@ -14924,7 +14921,7 @@
         <v>38107</v>
       </c>
       <c r="B47">
-        <v>3.9708686999999999E-2</v>
+        <v>44.46</v>
       </c>
       <c r="C47">
         <v>12181.397999999999</v>
@@ -14972,7 +14969,7 @@
         <v>4.25</v>
       </c>
       <c r="R47">
-        <v>-1.6790829419024988E-2</v>
+        <v>1107.3</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.35">
@@ -14980,7 +14977,7 @@
         <v>38138</v>
       </c>
       <c r="B48">
-        <v>-1.0127017E-2</v>
+        <v>47.13</v>
       </c>
       <c r="C48">
         <v>12181.397999999999</v>
@@ -15028,7 +15025,7 @@
         <v>4.07</v>
       </c>
       <c r="R48">
-        <v>1.2083446220536587E-2</v>
+        <v>1120.68</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.35">
@@ -15036,7 +15033,7 @@
         <v>38168</v>
       </c>
       <c r="B49">
-        <v>-8.8465460000000003E-3</v>
+        <v>48.2</v>
       </c>
       <c r="C49">
         <v>12181.397999999999</v>
@@ -15084,7 +15081,7 @@
         <v>4.01</v>
       </c>
       <c r="R49">
-        <v>1.7989078059749364E-2</v>
+        <v>1140.8399999999999</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.35">
@@ -15092,7 +15089,7 @@
         <v>38199</v>
       </c>
       <c r="B50">
-        <v>-7.2622870000000001E-3</v>
+        <v>44.02</v>
       </c>
       <c r="C50">
         <v>12367.744000000001</v>
@@ -15140,7 +15137,7 @@
         <v>4.08</v>
       </c>
       <c r="R50">
-        <v>-3.4290522772693732E-2</v>
+        <v>1101.72</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.35">
@@ -15148,7 +15145,7 @@
         <v>38230</v>
       </c>
       <c r="B51">
-        <v>-4.0045395999999997E-2</v>
+        <v>41.71</v>
       </c>
       <c r="C51">
         <v>12367.744000000001</v>
@@ -15196,7 +15193,7 @@
         <v>3.87</v>
       </c>
       <c r="R51">
-        <v>2.2873325345822426E-3</v>
+        <v>1104.24</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.35">
@@ -15204,7 +15201,7 @@
         <v>38260</v>
       </c>
       <c r="B52">
-        <v>-2.9097960000000001E-3</v>
+        <v>42.97</v>
       </c>
       <c r="C52">
         <v>12367.744000000001</v>
@@ -15252,7 +15249,7 @@
         <v>3.73</v>
       </c>
       <c r="R52">
-        <v>9.3639063971600045E-3</v>
+        <v>1114.58</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.35">
@@ -15260,7 +15257,7 @@
         <v>38291</v>
       </c>
       <c r="B53">
-        <v>-4.1227526E-2</v>
+        <v>45.44</v>
       </c>
       <c r="C53">
         <v>12562.163</v>
@@ -15308,7 +15305,7 @@
         <v>3.29</v>
       </c>
       <c r="R53">
-        <v>1.4014247519245071E-2</v>
+        <v>1130.2</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.35">
@@ -15316,7 +15313,7 @@
         <v>38321</v>
       </c>
       <c r="B54">
-        <v>-4.1307577999999998E-2</v>
+        <v>47.95</v>
       </c>
       <c r="C54">
         <v>12562.163</v>
@@ -15364,7 +15361,7 @@
         <v>3.1</v>
       </c>
       <c r="R54">
-        <v>3.8594938948858459E-2</v>
+        <v>1173.82</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.35">
@@ -15372,7 +15369,7 @@
         <v>38352</v>
       </c>
       <c r="B55">
-        <v>-2.0378456999999999E-2</v>
+        <v>48.46</v>
       </c>
       <c r="C55">
         <v>12562.163</v>
@@ -15420,7 +15417,7 @@
         <v>3.2</v>
       </c>
       <c r="R55">
-        <v>3.2458128162750732E-2</v>
+        <v>1211.92</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.35">
@@ -15428,7 +15425,7 @@
         <v>38383</v>
       </c>
       <c r="B56">
-        <v>-1.4064294E-2</v>
+        <v>45.61</v>
       </c>
       <c r="C56">
         <v>12813.728999999999</v>
@@ -15476,7 +15473,7 @@
         <v>3.05</v>
       </c>
       <c r="R56">
-        <v>-2.5290448214403627E-2</v>
+        <v>1181.27</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.35">
@@ -15484,7 +15481,7 @@
         <v>38411</v>
       </c>
       <c r="B57">
-        <v>-2.1210844E-2</v>
+        <v>45.86</v>
       </c>
       <c r="C57">
         <v>12813.728999999999</v>
@@ -15532,7 +15529,7 @@
         <v>2.98</v>
       </c>
       <c r="R57">
-        <v>1.8903383646414307E-2</v>
+        <v>1203.5999999999999</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.35">
@@ -15540,7 +15537,7 @@
         <v>38442</v>
       </c>
       <c r="B58">
-        <v>-1.402721E-3</v>
+        <v>44.8</v>
       </c>
       <c r="C58">
         <v>12813.728999999999</v>
@@ -15588,7 +15585,7 @@
         <v>3.78</v>
       </c>
       <c r="R58">
-        <v>-1.9117647058823573E-2</v>
+        <v>1180.5899999999999</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.35">
@@ -15596,7 +15593,7 @@
         <v>38472</v>
       </c>
       <c r="B59">
-        <v>-2.3692139000000001E-2</v>
+        <v>42.9</v>
       </c>
       <c r="C59">
         <v>12974.083000000001</v>
@@ -15644,7 +15641,7 @@
         <v>4.2300000000000004</v>
       </c>
       <c r="R59">
-        <v>-2.010858977291019E-2</v>
+        <v>1156.8499999999999</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.35">
@@ -15652,7 +15649,7 @@
         <v>38503</v>
       </c>
       <c r="B60">
-        <v>-1.2442521E-2</v>
+        <v>46.81</v>
       </c>
       <c r="C60">
         <v>12974.083000000001</v>
@@ -15700,7 +15697,7 @@
         <v>3.9</v>
       </c>
       <c r="R60">
-        <v>2.9952024895189666E-2</v>
+        <v>1191.5</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.35">
@@ -15708,7 +15705,7 @@
         <v>38533</v>
       </c>
       <c r="B61">
-        <v>-4.4085326000000001E-2</v>
+        <v>45.77</v>
       </c>
       <c r="C61">
         <v>12974.083000000001</v>
@@ -15756,7 +15753,7 @@
         <v>3.49</v>
       </c>
       <c r="R61">
-        <v>-1.4267729752415192E-4</v>
+        <v>1191.33</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.35">
@@ -15764,7 +15761,7 @@
         <v>38564</v>
       </c>
       <c r="B62">
-        <v>-2.0514119000000001E-2</v>
+        <v>48.67</v>
       </c>
       <c r="C62">
         <v>13205.445</v>
@@ -15812,7 +15809,7 @@
         <v>3.37</v>
       </c>
       <c r="R62">
-        <v>3.5968203604375137E-2</v>
+        <v>1234.18</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.35">
@@ -15820,7 +15817,7 @@
         <v>38595</v>
       </c>
       <c r="B63">
-        <v>-8.5373510000000003E-3</v>
+        <v>48.33</v>
       </c>
       <c r="C63">
         <v>13205.445</v>
@@ -15868,7 +15865,7 @@
         <v>3.64</v>
       </c>
       <c r="R63">
-        <v>-1.1222025960556881E-2</v>
+        <v>1220.33</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.35">
@@ -15876,7 +15873,7 @@
         <v>38625</v>
       </c>
       <c r="B64">
-        <v>-3.0314098000000001E-2</v>
+        <v>48.64</v>
       </c>
       <c r="C64">
         <v>13205.445</v>
@@ -15924,7 +15921,7 @@
         <v>3.58</v>
       </c>
       <c r="R64">
-        <v>6.9489400408087043E-3</v>
+        <v>1228.81</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.35">
@@ -15932,7 +15929,7 @@
         <v>38656</v>
       </c>
       <c r="B65">
-        <v>7.5834971000000001E-2</v>
+        <v>47.46</v>
       </c>
       <c r="C65">
         <v>13381.629000000001</v>
@@ -15980,7 +15977,7 @@
         <v>3.62</v>
       </c>
       <c r="R65">
-        <v>-1.7740741042146402E-2</v>
+        <v>1207.01</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.35">
@@ -15988,7 +15985,7 @@
         <v>38686</v>
       </c>
       <c r="B66">
-        <v>5.2417800000000004E-4</v>
+        <v>51</v>
       </c>
       <c r="C66">
         <v>13381.629000000001</v>
@@ -16036,7 +16033,7 @@
         <v>3.65</v>
       </c>
       <c r="R66">
-        <v>3.518612107604735E-2</v>
+        <v>1249.48</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.35">
@@ -16044,7 +16041,7 @@
         <v>38717</v>
       </c>
       <c r="B67">
-        <v>-1.96181E-3</v>
+        <v>49.72</v>
       </c>
       <c r="C67">
         <v>13381.629000000001</v>
@@ -16092,7 +16089,7 @@
         <v>3.55</v>
       </c>
       <c r="R67">
-        <v>-9.5239619681797283E-4</v>
+        <v>1248.29</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.35">
@@ -16100,7 +16097,7 @@
         <v>38748</v>
       </c>
       <c r="B68">
-        <v>-2.4993623999999999E-2</v>
+        <v>51.79</v>
       </c>
       <c r="C68">
         <v>13648.904</v>
@@ -16148,7 +16145,7 @@
         <v>3.34</v>
       </c>
       <c r="R68">
-        <v>2.5466838635253009E-2</v>
+        <v>1280.08</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.35">
@@ -16156,7 +16153,7 @@
         <v>38776</v>
       </c>
       <c r="B69">
-        <v>-8.847321E-3</v>
+        <v>51.14</v>
       </c>
       <c r="C69">
         <v>13648.904</v>
@@ -16204,7 +16201,7 @@
         <v>3.25</v>
       </c>
       <c r="R69">
-        <v>4.5309668145754323E-4</v>
+        <v>1280.6600000000001</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.35">
@@ -16212,7 +16209,7 @@
         <v>38807</v>
       </c>
       <c r="B70">
-        <v>4.6145709E-2</v>
+        <v>52.260100000000001</v>
       </c>
       <c r="C70">
         <v>13648.904</v>
@@ -16260,7 +16257,7 @@
         <v>3.06</v>
       </c>
       <c r="R70">
-        <v>1.1064607311854768E-2</v>
+        <v>1294.83</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.35">
@@ -16268,7 +16265,7 @@
         <v>38837</v>
       </c>
       <c r="B71">
-        <v>-1.4207508000000001E-2</v>
+        <v>51.94</v>
       </c>
       <c r="C71">
         <v>13799.794</v>
@@ -16316,7 +16313,7 @@
         <v>3.02</v>
       </c>
       <c r="R71">
-        <v>1.2186928013716125E-2</v>
+        <v>1310.6099999999999</v>
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.35">
@@ -16324,7 +16321,7 @@
         <v>38868</v>
       </c>
       <c r="B72">
-        <v>-1.2866700999999999E-2</v>
+        <v>47.99</v>
       </c>
       <c r="C72">
         <v>13799.794</v>
@@ -16372,7 +16369,7 @@
         <v>3.28</v>
       </c>
       <c r="R72">
-        <v>-3.091690129023883E-2</v>
+        <v>1270.0899999999999</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.35">
@@ -16380,7 +16377,7 @@
         <v>38898</v>
       </c>
       <c r="B73">
-        <v>-1.6824794000000001E-2</v>
+        <v>47.46</v>
       </c>
       <c r="C73">
         <v>13799.794</v>
@@ -16428,7 +16425,7 @@
         <v>3.37</v>
       </c>
       <c r="R73">
-        <v>8.6608035651192239E-5</v>
+        <v>1270.2</v>
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.35">
@@ -16436,7 +16433,7 @@
         <v>38929</v>
       </c>
       <c r="B74">
-        <v>-4.5174538E-2</v>
+        <v>45.74</v>
       </c>
       <c r="C74">
         <v>13908.498</v>
@@ -16484,7 +16481,7 @@
         <v>3.42</v>
       </c>
       <c r="R74">
-        <v>5.0858132577547011E-3</v>
+        <v>1276.6600000000001</v>
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.35">
@@ -16492,7 +16489,7 @@
         <v>38960</v>
       </c>
       <c r="B75">
-        <v>-2.7144536E-2</v>
+        <v>49.39</v>
       </c>
       <c r="C75">
         <v>13908.498</v>
@@ -16540,7 +16537,7 @@
         <v>3.43</v>
       </c>
       <c r="R75">
-        <v>2.1274262528785837E-2</v>
+        <v>1303.82</v>
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.35">
@@ -16548,7 +16545,7 @@
         <v>38990</v>
       </c>
       <c r="B76">
-        <v>2.6785713999999999E-2</v>
+        <v>51.35</v>
       </c>
       <c r="C76">
         <v>13908.498</v>
@@ -16596,7 +16593,7 @@
         <v>3.25</v>
       </c>
       <c r="R76">
-        <v>2.4566274485741779E-2</v>
+        <v>1335.85</v>
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.35">
@@ -16604,7 +16601,7 @@
         <v>39021</v>
       </c>
       <c r="B77">
-        <v>-5.0630011000000003E-2</v>
+        <v>53.17</v>
       </c>
       <c r="C77">
         <v>14066.37</v>
@@ -16652,7 +16649,7 @@
         <v>3.14</v>
       </c>
       <c r="R77">
-        <v>3.1508028596025195E-2</v>
+        <v>1377.94</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.35">
@@ -16660,7 +16657,7 @@
         <v>39051</v>
       </c>
       <c r="B78">
-        <v>-2.4035773999999999E-2</v>
+        <v>55.22</v>
       </c>
       <c r="C78">
         <v>14066.37</v>
@@ -16708,7 +16705,7 @@
         <v>3</v>
       </c>
       <c r="R78">
-        <v>1.6466609576614388E-2</v>
+        <v>1400.63</v>
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.35">
@@ -16716,7 +16713,7 @@
         <v>39082</v>
       </c>
       <c r="B79">
-        <v>-4.673417E-3</v>
+        <v>54.45</v>
       </c>
       <c r="C79">
         <v>14066.37</v>
@@ -16764,7 +16761,7 @@
         <v>2.76</v>
       </c>
       <c r="R79">
-        <v>1.2615751483260995E-2</v>
+        <v>1418.3</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.35">
@@ -16772,7 +16769,7 @@
         <v>39113</v>
       </c>
       <c r="B80">
-        <v>2.7895559999999999E-3</v>
+        <v>55.33</v>
       </c>
       <c r="C80">
         <v>14233.226000000001</v>
@@ -16820,7 +16817,7 @@
         <v>2.62</v>
       </c>
       <c r="R80">
-        <v>1.4059084819854739E-2</v>
+        <v>1438.24</v>
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.35">
@@ -16828,7 +16825,7 @@
         <v>39141</v>
       </c>
       <c r="B81">
-        <v>-4.3236894999999997E-2</v>
+        <v>53.82</v>
       </c>
       <c r="C81">
         <v>14233.226000000001</v>
@@ -16876,7 +16873,7 @@
         <v>2.86</v>
       </c>
       <c r="R81">
-        <v>-2.1846145288686225E-2</v>
+        <v>1406.82</v>
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.35">
@@ -16884,7 +16881,7 @@
         <v>39172</v>
       </c>
       <c r="B82">
-        <v>-3.5423745999999999E-2</v>
+        <v>53.95</v>
       </c>
       <c r="C82">
         <v>14233.226000000001</v>
@@ -16932,7 +16929,7 @@
         <v>2.74</v>
       </c>
       <c r="R82">
-        <v>9.9799547916576969E-3</v>
+        <v>1420.86</v>
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.35">
@@ -16940,7 +16937,7 @@
         <v>39202</v>
       </c>
       <c r="B83">
-        <v>-3.8895486999999999E-2</v>
+        <v>56.62</v>
       </c>
       <c r="C83">
         <v>14422.313</v>
@@ -16988,7 +16985,7 @@
         <v>2.57</v>
       </c>
       <c r="R83">
-        <v>4.3290683107413797E-2</v>
+        <v>1482.37</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.35">
@@ -16996,7 +16993,7 @@
         <v>39233</v>
       </c>
       <c r="B84">
-        <v>-9.3146389999999996E-3</v>
+        <v>59.04</v>
       </c>
       <c r="C84">
         <v>14422.313</v>
@@ -17044,7 +17041,7 @@
         <v>2.61</v>
       </c>
       <c r="R84">
-        <v>3.2549228600146973E-2</v>
+        <v>1530.62</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.35">
@@ -17052,7 +17049,7 @@
         <v>39263</v>
       </c>
       <c r="B85">
-        <v>5.9086188999999997E-2</v>
+        <v>59.52</v>
       </c>
       <c r="C85">
         <v>14422.313</v>
@@ -17100,7 +17097,7 @@
         <v>3.35</v>
       </c>
       <c r="R85">
-        <v>-1.7816309730697366E-2</v>
+        <v>1503.35</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.35">
@@ -17108,7 +17105,7 @@
         <v>39294</v>
       </c>
       <c r="B86">
-        <v>4.0518639000000002E-2</v>
+        <v>58.89</v>
       </c>
       <c r="C86">
         <v>14569.674999999999</v>
@@ -17156,7 +17153,7 @@
         <v>4.3099999999999996</v>
       </c>
       <c r="R86">
-        <v>-3.1981907074200899E-2</v>
+        <v>1455.27</v>
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.35">
@@ -17164,7 +17161,7 @@
         <v>39325</v>
       </c>
       <c r="B87">
-        <v>-1.7515923999999999E-2</v>
+        <v>60.57</v>
       </c>
       <c r="C87">
         <v>14569.674999999999</v>
@@ -17212,7 +17209,7 @@
         <v>4.42</v>
       </c>
       <c r="R87">
-        <v>1.2863592323073991E-2</v>
+        <v>1473.99</v>
       </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.35">
@@ -17220,7 +17217,7 @@
         <v>39355</v>
       </c>
       <c r="B88">
-        <v>-2.7863776999999999E-2</v>
+        <v>62.8</v>
       </c>
       <c r="C88">
         <v>14569.674999999999</v>
@@ -17268,7 +17265,7 @@
         <v>4.16</v>
       </c>
       <c r="R88">
-        <v>3.579400131615551E-2</v>
+        <v>1526.75</v>
       </c>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.35">
@@ -17276,7 +17273,7 @@
         <v>39386</v>
       </c>
       <c r="B89">
-        <v>-5.9679767000000002E-2</v>
+        <v>67.09</v>
       </c>
       <c r="C89">
         <v>14685.33</v>
@@ -17324,7 +17321,7 @@
         <v>5.31</v>
       </c>
       <c r="R89">
-        <v>1.4822335025380884E-2</v>
+        <v>1549.38</v>
       </c>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.35">
@@ -17332,7 +17329,7 @@
         <v>39416</v>
       </c>
       <c r="B90">
-        <v>2.919708E-3</v>
+        <v>61.75</v>
       </c>
       <c r="C90">
         <v>14685.33</v>
@@ -17380,7 +17377,7 @@
         <v>5.69</v>
       </c>
       <c r="R90">
-        <v>-4.4043423821141348E-2</v>
+        <v>1481.14</v>
       </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.35">
@@ -17388,7 +17385,7 @@
         <v>39447</v>
       </c>
       <c r="B91">
-        <v>3.3199879999999998E-3</v>
+        <v>62.46</v>
       </c>
       <c r="C91">
         <v>14685.33</v>
@@ -17436,7 +17433,7 @@
         <v>6.8</v>
       </c>
       <c r="R91">
-        <v>-8.628488866683881E-3</v>
+        <v>1468.36</v>
       </c>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.35">
@@ -17444,7 +17441,7 @@
         <v>39478</v>
       </c>
       <c r="B92">
-        <v>7.4042998999999998E-2</v>
+        <v>54.38</v>
       </c>
       <c r="C92">
         <v>14668.445</v>
@@ -17492,7 +17489,7 @@
         <v>7.25</v>
       </c>
       <c r="R92">
-        <v>-6.1163474897164116E-2</v>
+        <v>1378.55</v>
       </c>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.35">
@@ -17500,7 +17497,7 @@
         <v>39507</v>
       </c>
       <c r="B93">
-        <v>3.3940577E-2</v>
+        <v>52.4</v>
       </c>
       <c r="C93">
         <v>14668.445</v>
@@ -17548,7 +17545,7 @@
         <v>8.08</v>
       </c>
       <c r="R93">
-        <v>-3.4761162090602316E-2</v>
+        <v>1330.63</v>
       </c>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.35">
@@ -17556,7 +17553,7 @@
         <v>39538</v>
       </c>
       <c r="B94">
-        <v>2.9363779999999999E-3</v>
+        <v>52.5</v>
       </c>
       <c r="C94">
         <v>14668.445</v>
@@ -17604,7 +17601,7 @@
         <v>7.39</v>
       </c>
       <c r="R94">
-        <v>-5.9595830546433914E-3</v>
+        <v>1322.7</v>
       </c>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.35">
@@ -17612,7 +17609,7 @@
         <v>39568</v>
       </c>
       <c r="B95">
-        <v>-5.5178791999999997E-2</v>
+        <v>56.43</v>
       </c>
       <c r="C95">
         <v>14812.974</v>
@@ -17660,7 +17657,7 @@
         <v>6.69</v>
       </c>
       <c r="R95">
-        <v>4.7546684811370588E-2</v>
+        <v>1385.59</v>
       </c>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.35">
@@ -17668,7 +17665,7 @@
         <v>39599</v>
       </c>
       <c r="B96">
-        <v>-3.3565045000000002E-2</v>
+        <v>59.96</v>
       </c>
       <c r="C96">
         <v>14812.974</v>
@@ -17716,7 +17713,7 @@
         <v>6.73</v>
       </c>
       <c r="R96">
-        <v>1.0674153248796614E-2</v>
+        <v>1400.38</v>
       </c>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.35">
@@ -17724,7 +17721,7 @@
         <v>39629</v>
       </c>
       <c r="B97">
-        <v>1.6042780999999999E-2</v>
+        <v>54.19</v>
       </c>
       <c r="C97">
         <v>14812.974</v>
@@ -17772,7 +17769,7 @@
         <v>7.75</v>
       </c>
       <c r="R97">
-        <v>-8.5962381639269392E-2</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.35">
@@ -17780,7 +17777,7 @@
         <v>39660</v>
       </c>
       <c r="B98">
-        <v>7.5996092000000001E-2</v>
+        <v>53.49</v>
       </c>
       <c r="C98">
         <v>14842.983</v>
@@ -17828,7 +17825,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="R98">
-        <v>-9.8593749999998925E-3</v>
+        <v>1267.3800000000001</v>
       </c>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.35">
@@ -17836,7 +17833,7 @@
         <v>39691</v>
       </c>
       <c r="B99">
-        <v>7.6578050000000002E-3</v>
+        <v>54.8</v>
       </c>
       <c r="C99">
         <v>14842.983</v>
@@ -17884,7 +17881,7 @@
         <v>9.19</v>
       </c>
       <c r="R99">
-        <v>1.2190503242910378E-2</v>
+        <v>1282.83</v>
       </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.35">
@@ -17892,7 +17889,7 @@
         <v>39721</v>
       </c>
       <c r="B100">
-        <v>0.159436834</v>
+        <v>47.43</v>
       </c>
       <c r="C100">
         <v>14842.983</v>
@@ -17940,7 +17937,7 @@
         <v>14.94</v>
       </c>
       <c r="R100">
-        <v>-9.0791453271283018E-2</v>
+        <v>1166.3599999999999</v>
       </c>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.35">
@@ -17948,7 +17945,7 @@
         <v>39752</v>
       </c>
       <c r="B101">
-        <v>0.11861521</v>
+        <v>39.49</v>
       </c>
       <c r="C101">
         <v>14549.949000000001</v>
@@ -17996,7 +17993,7 @@
         <v>17.96</v>
       </c>
       <c r="R101">
-        <v>-0.16942453444905514</v>
+        <v>968.75</v>
       </c>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.35">
@@ -18004,7 +18001,7 @@
         <v>39782</v>
       </c>
       <c r="B102">
-        <v>-1.2054947999999999E-2</v>
+        <v>34.549999999999997</v>
       </c>
       <c r="C102">
         <v>14549.949000000001</v>
@@ -18052,7 +18049,7 @@
         <v>20.309999999999999</v>
       </c>
       <c r="R102">
-        <v>-7.4849032258064496E-2</v>
+        <v>896.24</v>
       </c>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.35">
@@ -18060,7 +18057,7 @@
         <v>39813</v>
       </c>
       <c r="B103">
-        <v>2.8695024999999999E-2</v>
+        <v>35.33</v>
       </c>
       <c r="C103">
         <v>14549.949000000001</v>
@@ -18108,7 +18105,7 @@
         <v>16.73</v>
       </c>
       <c r="R103">
-        <v>7.8215656520574939E-3</v>
+        <v>903.25</v>
       </c>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.35">
@@ -18116,7 +18113,7 @@
         <v>39844</v>
       </c>
       <c r="B104">
-        <v>1.1670313999999999E-2</v>
+        <v>34.35</v>
       </c>
       <c r="C104">
         <v>14383.885</v>
@@ -18164,7 +18161,7 @@
         <v>16.54</v>
       </c>
       <c r="R104">
-        <v>-8.5657348463880401E-2</v>
+        <v>825.88</v>
       </c>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.35">
@@ -18172,7 +18169,7 @@
         <v>39872</v>
       </c>
       <c r="B105">
-        <v>0.14383447399999999</v>
+        <v>33.15</v>
       </c>
       <c r="C105">
         <v>14383.885</v>
@@ -18220,7 +18217,7 @@
         <v>17.84</v>
       </c>
       <c r="R105">
-        <v>-0.10993122487528451</v>
+        <v>735.09</v>
       </c>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.35">
@@ -18228,7 +18225,7 @@
         <v>39903</v>
       </c>
       <c r="B106">
-        <v>-1.5280973E-2</v>
+        <v>37.03</v>
       </c>
       <c r="C106">
         <v>14383.885</v>
@@ -18276,7 +18273,7 @@
         <v>15.6</v>
       </c>
       <c r="R106">
-        <v>8.5404508291501591E-2</v>
+        <v>797.87</v>
       </c>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.35">
@@ -18284,7 +18281,7 @@
         <v>39933</v>
       </c>
       <c r="B107">
-        <v>-1.153159E-2</v>
+        <v>41.61</v>
       </c>
       <c r="C107">
         <v>14340.416999999999</v>
@@ -18332,7 +18329,7 @@
         <v>12.51</v>
       </c>
       <c r="R107">
-        <v>9.3925075513554779E-2</v>
+        <v>872.81</v>
       </c>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.35">
@@ -18340,7 +18337,7 @@
         <v>39964</v>
       </c>
       <c r="B108">
-        <v>-4.0068600000000003E-2</v>
+        <v>42.69</v>
       </c>
       <c r="C108">
         <v>14340.416999999999</v>
@@ -18388,7 +18385,7 @@
         <v>10.81</v>
       </c>
       <c r="R108">
-        <v>5.3081426656431674E-2</v>
+        <v>919.14</v>
       </c>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.35">
@@ -18396,7 +18393,7 @@
         <v>39994</v>
       </c>
       <c r="B109">
-        <v>-3.9964077000000001E-2</v>
+        <v>44.49</v>
       </c>
       <c r="C109">
         <v>14340.416999999999</v>
@@ -18444,7 +18441,7 @@
         <v>10.27</v>
       </c>
       <c r="R109">
-        <v>1.9583523728705643E-4</v>
+        <v>919.32</v>
       </c>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.35">
@@ -18452,7 +18449,7 @@
         <v>40025</v>
       </c>
       <c r="B110">
-        <v>-4.2743418999999998E-2</v>
+        <v>48.51</v>
       </c>
       <c r="C110">
         <v>14384.145</v>
@@ -18500,7 +18497,7 @@
         <v>8.9700000000000006</v>
       </c>
       <c r="R110">
-        <v>7.4141756950789617E-2</v>
+        <v>987.48</v>
       </c>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.35">
@@ -18508,7 +18505,7 @@
         <v>40056</v>
       </c>
       <c r="B111">
-        <v>-8.0557130000000008E-3</v>
+        <v>49.62</v>
       </c>
       <c r="C111">
         <v>14384.145</v>
@@ -18556,7 +18553,7 @@
         <v>8.4499999999999993</v>
       </c>
       <c r="R111">
-        <v>3.3560173370599911E-2</v>
+        <v>1020.62</v>
       </c>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.35">
@@ -18564,7 +18561,7 @@
         <v>40086</v>
       </c>
       <c r="B112">
-        <v>-4.5837810000000003E-3</v>
+        <v>51.95</v>
       </c>
       <c r="C112">
         <v>14384.145</v>
@@ -18612,7 +18609,7 @@
         <v>7.76</v>
       </c>
       <c r="R112">
-        <v>3.5723383825517763E-2</v>
+        <v>1057.08</v>
       </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.35">
@@ -18620,7 +18617,7 @@
         <v>40117</v>
       </c>
       <c r="B113">
-        <v>3.3845253999999998E-2</v>
+        <v>51.47</v>
       </c>
       <c r="C113">
         <v>14566.511</v>
@@ -18668,7 +18665,7 @@
         <v>7.56</v>
       </c>
       <c r="R113">
-        <v>-1.9761985847807084E-2</v>
+        <v>1036.19</v>
       </c>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.35">
@@ -18676,7 +18673,7 @@
         <v>40147</v>
       </c>
       <c r="B114">
-        <v>-4.2973124000000001E-2</v>
+        <v>54.12</v>
       </c>
       <c r="C114">
         <v>14566.511</v>
@@ -18724,7 +18721,7 @@
         <v>6.94</v>
       </c>
       <c r="R114">
-        <v>5.7363996950366314E-2</v>
+        <v>1095.6300000000001</v>
       </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.35">
@@ -18732,7 +18729,7 @@
         <v>40178</v>
       </c>
       <c r="B115">
-        <v>-4.4792085000000002E-2</v>
+        <v>57.54</v>
       </c>
       <c r="C115">
         <v>14566.511</v>
@@ -18780,7 +18777,7 @@
         <v>6.23</v>
       </c>
       <c r="R115">
-        <v>1.7770597738287375E-2</v>
+        <v>1115.0999999999999</v>
       </c>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.35">
@@ -18788,7 +18785,7 @@
         <v>40209</v>
       </c>
       <c r="B116">
-        <v>4.6892496999999998E-2</v>
+        <v>52.49</v>
       </c>
       <c r="C116">
         <v>14681.063</v>
@@ -18836,7 +18833,7 @@
         <v>6.73</v>
       </c>
       <c r="R116">
-        <v>-3.6974262397991176E-2</v>
+        <v>1073.8699999999999</v>
       </c>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.35">
@@ -18844,7 +18841,7 @@
         <v>40237</v>
       </c>
       <c r="B117">
-        <v>7.1589490000000004E-3</v>
+        <v>55.07</v>
       </c>
       <c r="C117">
         <v>14681.063</v>
@@ -18892,7 +18889,7 @@
         <v>6.12</v>
       </c>
       <c r="R117">
-        <v>2.8513693463827261E-2</v>
+        <v>1104.49</v>
       </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.35">
@@ -18900,7 +18897,7 @@
         <v>40268</v>
       </c>
       <c r="B118">
-        <v>-1.9189712000000001E-2</v>
+        <v>58.39</v>
       </c>
       <c r="C118">
         <v>14681.063</v>
@@ -18948,7 +18945,7 @@
         <v>5.59</v>
       </c>
       <c r="R118">
-        <v>5.8796367554255768E-2</v>
+        <v>1169.43</v>
       </c>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.35">
@@ -18956,7 +18953,7 @@
         <v>40298</v>
       </c>
       <c r="B119">
-        <v>-2.7041571E-2</v>
+        <v>59.56</v>
       </c>
       <c r="C119">
         <v>14888.6</v>
@@ -19004,7 +19001,7 @@
         <v>6.5</v>
       </c>
       <c r="R119">
-        <v>1.4759327193589966E-2</v>
+        <v>1186.69</v>
       </c>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.35">
@@ -19012,7 +19009,7 @@
         <v>40329</v>
       </c>
       <c r="B120">
-        <v>6.1705470999999998E-2</v>
+        <v>55.13</v>
       </c>
       <c r="C120">
         <v>14888.6</v>
@@ -19060,7 +19057,7 @@
         <v>7.02</v>
       </c>
       <c r="R120">
-        <v>-8.1975916203894883E-2</v>
+        <v>1089.4100000000001</v>
       </c>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.35">
@@ -19068,7 +19065,7 @@
         <v>40359</v>
       </c>
       <c r="B121">
-        <v>1.8475414999999999E-2</v>
+        <v>51.6</v>
       </c>
       <c r="C121">
         <v>14888.6</v>
@@ -19116,7 +19113,7 @@
         <v>6.78</v>
       </c>
       <c r="R121">
-        <v>-5.3882376699314394E-2</v>
+        <v>1030.71</v>
       </c>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.35">
@@ -19124,7 +19121,7 @@
         <v>40390</v>
       </c>
       <c r="B122">
-        <v>-6.7805803999999997E-2</v>
+        <v>55.44</v>
       </c>
       <c r="C122">
         <v>15057.66</v>
@@ -19172,7 +19169,7 @@
         <v>6.76</v>
       </c>
       <c r="R122">
-        <v>6.8777832756061308E-2</v>
+        <v>1101.5999999999999</v>
       </c>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.35">
@@ -19180,7 +19177,7 @@
         <v>40421</v>
       </c>
       <c r="B123">
-        <v>-1.0068466E-2</v>
+        <v>51.54</v>
       </c>
       <c r="C123">
         <v>15057.66</v>
@@ -19228,7 +19225,7 @@
         <v>6.42</v>
       </c>
       <c r="R123">
-        <v>-4.7449164851125603E-2</v>
+        <v>1049.33</v>
       </c>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.35">
@@ -19236,7 +19233,7 @@
         <v>40451</v>
       </c>
       <c r="B124">
-        <v>-2.2697454999999998E-2</v>
+        <v>57.85</v>
       </c>
       <c r="C124">
         <v>15057.66</v>
@@ -19284,7 +19281,7 @@
         <v>6.01</v>
       </c>
       <c r="R124">
-        <v>8.7551104037814742E-2</v>
+        <v>1141.2</v>
       </c>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.35">
@@ -19292,7 +19289,7 @@
         <v>40482</v>
       </c>
       <c r="B125">
-        <v>-1.5627017999999999E-2</v>
+        <v>61.67</v>
       </c>
       <c r="C125">
         <v>15230.208000000001</v>
@@ -19340,7 +19337,7 @@
         <v>5.87</v>
       </c>
       <c r="R125">
-        <v>3.6855941114616098E-2</v>
+        <v>1183.26</v>
       </c>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.35">
@@ -19348,7 +19345,7 @@
         <v>40512</v>
       </c>
       <c r="B126">
-        <v>2.5834658E-2</v>
+        <v>60.94</v>
       </c>
       <c r="C126">
         <v>15230.208000000001</v>
@@ -19396,7 +19393,7 @@
         <v>5.55</v>
       </c>
       <c r="R126">
-        <v>-2.2902827780877377E-3</v>
+        <v>1180.55</v>
       </c>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.35">
@@ -19404,7 +19401,7 @@
         <v>40543</v>
       </c>
       <c r="B127">
-        <v>-2.1011673000000002E-2</v>
+        <v>64.38</v>
       </c>
       <c r="C127">
         <v>15230.208000000001</v>
@@ -19452,7 +19449,7 @@
         <v>5.12</v>
       </c>
       <c r="R127">
-        <v>6.5300072000338938E-2</v>
+        <v>1257.6400000000001</v>
       </c>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.35">
@@ -19460,7 +19457,7 @@
         <v>40574</v>
       </c>
       <c r="B128">
-        <v>-1.5199898E-2</v>
+        <v>66.930000000000007</v>
       </c>
       <c r="C128">
         <v>15238.370999999999</v>
@@ -19508,7 +19505,7 @@
         <v>4.66</v>
       </c>
       <c r="R128">
-        <v>2.2645590152984729E-2</v>
+        <v>1286.1199999999999</v>
       </c>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.35">
@@ -19516,7 +19513,7 @@
         <v>40602</v>
       </c>
       <c r="B129">
-        <v>-1.6210103E-2</v>
+        <v>68.31</v>
       </c>
       <c r="C129">
         <v>15238.370999999999</v>
@@ -19564,7 +19561,7 @@
         <v>4.84</v>
       </c>
       <c r="R129">
-        <v>3.1956582589494076E-2</v>
+        <v>1327.22</v>
       </c>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.35">
@@ -19572,7 +19569,7 @@
         <v>40633</v>
       </c>
       <c r="B130">
-        <v>2.7721769999999998E-3</v>
+        <v>66.540000000000006</v>
       </c>
       <c r="C130">
         <v>15238.370999999999</v>
@@ -19620,7 +19617,7 @@
         <v>4.66</v>
       </c>
       <c r="R130">
-        <v>-1.0473018791158362E-3</v>
+        <v>1325.83</v>
       </c>
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.35">
@@ -19628,7 +19625,7 @@
         <v>40663</v>
       </c>
       <c r="B131">
-        <v>-3.7593985000000003E-2</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="C131">
         <v>15460.925999999999</v>
@@ -19676,7 +19673,7 @@
         <v>4.8499999999999996</v>
       </c>
       <c r="R131">
-        <v>2.8495357625034856E-2</v>
+        <v>1363.61</v>
       </c>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.35">
@@ -19684,7 +19681,7 @@
         <v>40694</v>
       </c>
       <c r="B132">
-        <v>-1.3990195E-2</v>
+        <v>67.180000000000007</v>
       </c>
       <c r="C132">
         <v>15460.925999999999</v>
@@ -19732,7 +19729,7 @@
         <v>5.49</v>
       </c>
       <c r="R132">
-        <v>-1.350092768460176E-2</v>
+        <v>1345.2</v>
       </c>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.35">
@@ -19740,7 +19737,7 @@
         <v>40724</v>
       </c>
       <c r="B133">
-        <v>1.1490082E-2</v>
+        <v>65.02</v>
       </c>
       <c r="C133">
         <v>15460.925999999999</v>
@@ -19788,7 +19785,7 @@
         <v>5.43</v>
       </c>
       <c r="R133">
-        <v>-1.8257508177222714E-2</v>
+        <v>1320.64</v>
       </c>
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.35">
@@ -19796,7 +19793,7 @@
         <v>40755</v>
       </c>
       <c r="B134">
-        <v>1.1499878E-2</v>
+        <v>65.73</v>
       </c>
       <c r="C134">
         <v>15587.125</v>
@@ -19844,7 +19841,7 @@
         <v>6.99</v>
       </c>
       <c r="R134">
-        <v>-2.1474436636782279E-2</v>
+        <v>1292.28</v>
       </c>
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.35">
@@ -19852,7 +19849,7 @@
         <v>40786</v>
       </c>
       <c r="B135">
-        <v>-1.4943359999999999E-2</v>
+        <v>61.36</v>
       </c>
       <c r="C135">
         <v>15587.125</v>
@@ -19900,7 +19897,7 @@
         <v>7.68</v>
       </c>
       <c r="R135">
-        <v>-5.6791097904478782E-2</v>
+        <v>1218.8900000000001</v>
       </c>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.35">
@@ -19908,7 +19905,7 @@
         <v>40816</v>
       </c>
       <c r="B136">
-        <v>1.5045872E-2</v>
+        <v>59.14</v>
       </c>
       <c r="C136">
         <v>15587.125</v>
@@ -19956,7 +19953,7 @@
         <v>7.91</v>
       </c>
       <c r="R136">
-        <v>-7.1762012979021961E-2</v>
+        <v>1131.42</v>
       </c>
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.35">
@@ -19964,7 +19961,7 @@
         <v>40847</v>
       </c>
       <c r="B137">
-        <v>-4.1617819E-2</v>
+        <v>66.14</v>
       </c>
       <c r="C137">
         <v>15785.312</v>
@@ -20012,7 +20009,7 @@
         <v>7.61</v>
       </c>
       <c r="R137">
-        <v>0.10772303830584562</v>
+        <v>1253.3</v>
       </c>
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.35">
@@ -20020,7 +20017,7 @@
         <v>40877</v>
       </c>
       <c r="B138">
-        <v>-8.9462069999999994E-3</v>
+        <v>64.78</v>
       </c>
       <c r="C138">
         <v>15785.312</v>
@@ -20068,7 +20065,7 @@
         <v>7.52</v>
       </c>
       <c r="R138">
-        <v>-5.0586451767333784E-3</v>
+        <v>1246.96</v>
       </c>
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.35">
@@ -20076,7 +20073,7 @@
         <v>40908</v>
       </c>
       <c r="B139">
-        <v>-2.5475543E-2</v>
+        <v>63.9</v>
       </c>
       <c r="C139">
         <v>15785.312</v>
@@ -20124,7 +20121,7 @@
         <v>6.84</v>
       </c>
       <c r="R139">
-        <v>8.5327516520175006E-3</v>
+        <v>1257.5999999999999</v>
       </c>
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.35">
@@ -20132,7 +20129,7 @@
         <v>40939</v>
       </c>
       <c r="B140">
-        <v>3.4434293999999997E-2</v>
+        <v>69.19</v>
       </c>
       <c r="C140">
         <v>15973.880999999999</v>
@@ -20180,7 +20177,7 @@
         <v>6.24</v>
       </c>
       <c r="R140">
-        <v>4.3583015267175673E-2</v>
+        <v>1312.41</v>
       </c>
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.35">
@@ -20188,7 +20185,7 @@
         <v>40968</v>
       </c>
       <c r="B141">
-        <v>-6.0535509999999999E-3</v>
+        <v>74.17</v>
       </c>
       <c r="C141">
         <v>15973.880999999999</v>
@@ -20236,7 +20233,7 @@
         <v>5.96</v>
       </c>
       <c r="R141">
-        <v>4.0589449943234213E-2</v>
+        <v>1365.68</v>
       </c>
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.35">
@@ -20244,7 +20241,7 @@
         <v>40999</v>
       </c>
       <c r="B142">
-        <v>-3.0176420000000001E-3</v>
+        <v>77.81</v>
       </c>
       <c r="C142">
         <v>15973.880999999999</v>
@@ -20292,7 +20289,7 @@
         <v>6.13</v>
       </c>
       <c r="R142">
-        <v>3.1332376545017748E-2</v>
+        <v>1408.47</v>
       </c>
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.35">
@@ -20300,7 +20297,7 @@
         <v>41029</v>
       </c>
       <c r="B143">
-        <v>-1.5764222000000001E-2</v>
+        <v>75.709999999999994</v>
       </c>
       <c r="C143">
         <v>16121.851000000001</v>
@@ -20348,7 +20345,7 @@
         <v>6.31</v>
       </c>
       <c r="R143">
-        <v>-7.497497284287169E-3</v>
+        <v>1397.91</v>
       </c>
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.35">
@@ -20356,7 +20353,7 @@
         <v>41060</v>
       </c>
       <c r="B144">
-        <v>9.0097099999999998E-4</v>
+        <v>69.650000000000006</v>
       </c>
       <c r="C144">
         <v>16121.851000000001</v>
@@ -20404,7 +20401,7 @@
         <v>6.77</v>
       </c>
       <c r="R144">
-        <v>-6.2650671359386623E-2</v>
+        <v>1310.33</v>
       </c>
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.35">
@@ -20412,7 +20409,7 @@
         <v>41090</v>
       </c>
       <c r="B145">
-        <v>-2.8748473E-2</v>
+        <v>71.23</v>
       </c>
       <c r="C145">
         <v>16121.851000000001</v>
@@ -20460,7 +20457,7 @@
         <v>6.36</v>
       </c>
       <c r="R145">
-        <v>3.9554921279372435E-2</v>
+        <v>1362.16</v>
       </c>
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.35">
@@ -20468,7 +20465,7 @@
         <v>41121</v>
       </c>
       <c r="B146">
-        <v>-2.8167494000000001E-2</v>
+        <v>71.52</v>
       </c>
       <c r="C146">
         <v>16227.939</v>
@@ -20516,7 +20513,7 @@
         <v>5.92</v>
       </c>
       <c r="R146">
-        <v>1.2597639043871345E-2</v>
+        <v>1379.32</v>
       </c>
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.35">
@@ -20524,7 +20521,7 @@
         <v>41152</v>
       </c>
       <c r="B147">
-        <v>4.1123595999999998E-2</v>
+        <v>75.39</v>
       </c>
       <c r="C147">
         <v>16227.939</v>
@@ -20572,7 +20569,7 @@
         <v>5.61</v>
       </c>
       <c r="R147">
-        <v>1.9763361656468303E-2</v>
+        <v>1406.58</v>
       </c>
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.35">
@@ -20580,7 +20577,7 @@
         <v>41182</v>
       </c>
       <c r="B148">
-        <v>-5.5865919999999996E-3</v>
+        <v>75.87</v>
       </c>
       <c r="C148">
         <v>16227.939</v>
@@ -20628,7 +20625,7 @@
         <v>5.49</v>
       </c>
       <c r="R148">
-        <v>2.4236090375236552E-2</v>
+        <v>1440.67</v>
       </c>
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.35">
@@ -20636,7 +20633,7 @@
         <v>41213</v>
       </c>
       <c r="B149">
-        <v>-1.0940435E-2</v>
+        <v>70.290000000000006</v>
       </c>
       <c r="C149">
         <v>16297.349</v>
@@ -20684,7 +20681,7 @@
         <v>5.71</v>
       </c>
       <c r="R149">
-        <v>-1.9789403541407791E-2</v>
+        <v>1412.16</v>
       </c>
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.35">
@@ -20692,7 +20689,7 @@
         <v>41243</v>
       </c>
       <c r="B150">
-        <v>3.9995402999999999E-2</v>
+        <v>70.86</v>
       </c>
       <c r="C150">
         <v>16297.349</v>
@@ -20740,7 +20737,7 @@
         <v>5.34</v>
       </c>
       <c r="R150">
-        <v>2.8467029231815655E-3</v>
+        <v>1416.18</v>
       </c>
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.35">
@@ -20748,7 +20745,7 @@
         <v>41274</v>
       </c>
       <c r="B151">
-        <v>7.5266329999999996E-3</v>
+        <v>70.72</v>
       </c>
       <c r="C151">
         <v>16297.349</v>
@@ -20796,7 +20793,7 @@
         <v>4.92</v>
       </c>
       <c r="R151">
-        <v>7.0683105254980561E-3</v>
+        <v>1426.19</v>
       </c>
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.35">
@@ -20804,7 +20801,7 @@
         <v>41305</v>
       </c>
       <c r="B152">
-        <v>-4.8374656000000002E-2</v>
+        <v>71.73</v>
       </c>
       <c r="C152">
         <v>16475.439999999999</v>
@@ -20852,7 +20849,7 @@
         <v>4.99</v>
       </c>
       <c r="R152">
-        <v>5.0428063581991145E-2</v>
+        <v>1498.11</v>
       </c>
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.35">
@@ -20860,7 +20857,7 @@
         <v>41333</v>
       </c>
       <c r="B153">
-        <v>-2.2617123999999999E-2</v>
+        <v>71.849999999999994</v>
       </c>
       <c r="C153">
         <v>16475.439999999999</v>
@@ -20908,7 +20905,7 @@
         <v>4.8</v>
       </c>
       <c r="R153">
-        <v>1.1060603026480154E-2</v>
+        <v>1514.68</v>
       </c>
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.35">
@@ -20916,7 +20913,7 @@
         <v>41364</v>
       </c>
       <c r="B154">
-        <v>-4.3769309999999999E-2</v>
+        <v>73.31</v>
       </c>
       <c r="C154">
         <v>16475.439999999999</v>
@@ -20964,7 +20961,7 @@
         <v>4.76</v>
       </c>
       <c r="R154">
-        <v>3.5987799403174314E-2</v>
+        <v>1569.19</v>
       </c>
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.35">
@@ -20972,7 +20969,7 @@
         <v>41394</v>
       </c>
       <c r="B155">
-        <v>-5.2960108999999998E-2</v>
+        <v>73.63</v>
       </c>
       <c r="C155">
         <v>16541.39</v>
@@ -21020,7 +21017,7 @@
         <v>4.38</v>
       </c>
       <c r="R155">
-        <v>1.8085763992887971E-2</v>
+        <v>1597.57</v>
       </c>
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.35">
@@ -21028,7 +21025,7 @@
         <v>41425</v>
       </c>
       <c r="B156">
-        <v>8.7505303000000006E-2</v>
+        <v>76.77</v>
       </c>
       <c r="C156">
         <v>16541.39</v>
@@ -21076,7 +21073,7 @@
         <v>5.0599999999999996</v>
       </c>
       <c r="R156">
-        <v>2.0762783477406455E-2</v>
+        <v>1630.74</v>
       </c>
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.35">
@@ -21084,7 +21081,7 @@
         <v>41455</v>
       </c>
       <c r="B157">
-        <v>-3.1719180000000001E-3</v>
+        <v>73.63</v>
       </c>
       <c r="C157">
         <v>16541.39</v>
@@ -21132,7 +21129,7 @@
         <v>4.82</v>
       </c>
       <c r="R157">
-        <v>-1.499932545960736E-2</v>
+        <v>1606.28</v>
       </c>
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.35">
@@ -21140,7 +21137,7 @@
         <v>41486</v>
       </c>
       <c r="B158">
-        <v>-4.1062557E-2</v>
+        <v>77.25</v>
       </c>
       <c r="C158">
         <v>16749.348999999998</v>
@@ -21188,7 +21185,7 @@
         <v>4.75</v>
       </c>
       <c r="R158">
-        <v>4.9462111213487203E-2</v>
+        <v>1685.73</v>
       </c>
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.35">
@@ -21196,7 +21193,7 @@
         <v>41517</v>
       </c>
       <c r="B159">
-        <v>5.5995717E-2</v>
+        <v>76.77</v>
       </c>
       <c r="C159">
         <v>16749.348999999998</v>
@@ -21244,7 +21241,7 @@
         <v>4.6399999999999997</v>
       </c>
       <c r="R159">
-        <v>-3.1298013323604601E-2</v>
+        <v>1632.97</v>
       </c>
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.35">
@@ -21252,7 +21249,7 @@
         <v>41547</v>
       </c>
       <c r="B160">
-        <v>-5.2188729999999997E-3</v>
+        <v>78.8</v>
       </c>
       <c r="C160">
         <v>16749.348999999998</v>
@@ -21300,7 +21297,7 @@
         <v>4.55</v>
       </c>
       <c r="R160">
-        <v>2.9749474883188354E-2</v>
+        <v>1681.55</v>
       </c>
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.35">
@@ -21308,7 +21305,7 @@
         <v>41578</v>
       </c>
       <c r="B161">
-        <v>-3.7124397000000003E-2</v>
+        <v>82.281999999999996</v>
       </c>
       <c r="C161">
         <v>16999.887999999999</v>
@@ -21356,7 +21353,7 @@
         <v>4.32</v>
       </c>
       <c r="R161">
-        <v>4.4595759864410889E-2</v>
+        <v>1756.54</v>
       </c>
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.35">
@@ -21364,7 +21361,7 @@
         <v>41608</v>
       </c>
       <c r="B162">
-        <v>2.1260997E-2</v>
+        <v>85.2</v>
       </c>
       <c r="C162">
         <v>16999.887999999999</v>
@@ -21412,7 +21409,7 @@
         <v>4.09</v>
       </c>
       <c r="R162">
-        <v>2.804946087194149E-2</v>
+        <v>1805.81</v>
       </c>
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.35">
@@ -21420,7 +21417,7 @@
         <v>41639</v>
       </c>
       <c r="B163">
-        <v>-3.5483200000000002E-3</v>
+        <v>88.44</v>
       </c>
       <c r="C163">
         <v>16999.887999999999</v>
@@ -21468,7 +21465,7 @@
         <v>3.97</v>
       </c>
       <c r="R163">
-        <v>2.3562833299184183E-2</v>
+        <v>1848.36</v>
       </c>
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.35">
@@ -21476,7 +21473,7 @@
         <v>41670</v>
       </c>
       <c r="B164">
-        <v>-2.6516306E-2</v>
+        <v>86.93</v>
       </c>
       <c r="C164">
         <v>17031.324000000001</v>
@@ -21524,7 +21521,7 @@
         <v>4.03</v>
       </c>
       <c r="R164">
-        <v>-3.5582895107013734E-2</v>
+        <v>1782.59</v>
       </c>
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.35">
@@ -21532,7 +21529,7 @@
         <v>41698</v>
       </c>
       <c r="B165">
-        <v>-3.1296131999999997E-2</v>
+        <v>90.974000000000004</v>
       </c>
       <c r="C165">
         <v>17031.324000000001</v>
@@ -21580,7 +21577,7 @@
         <v>3.81</v>
       </c>
       <c r="R165">
-        <v>4.3117037568930705E-2</v>
+        <v>1859.45</v>
       </c>
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.35">
@@ -21588,7 +21585,7 @@
         <v>41729</v>
       </c>
       <c r="B166">
-        <v>-2.4762453E-2</v>
+        <v>91.06</v>
       </c>
       <c r="C166">
         <v>17031.324000000001</v>
@@ -21636,7 +21633,7 @@
         <v>3.71</v>
       </c>
       <c r="R166">
-        <v>6.9321573583585039E-3</v>
+        <v>1872.34</v>
       </c>
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.35">
@@ -21644,7 +21641,7 @@
         <v>41759</v>
       </c>
       <c r="B167">
-        <v>-3.7238958000000003E-2</v>
+        <v>90.88</v>
       </c>
       <c r="C167">
         <v>17320.920999999998</v>
@@ -21692,7 +21689,7 @@
         <v>3.75</v>
       </c>
       <c r="R167">
-        <v>6.2007968638175814E-3</v>
+        <v>1883.95</v>
       </c>
     </row>
     <row r="168" spans="1:18" x14ac:dyDescent="0.35">
@@ -21700,7 +21697,7 @@
         <v>41790</v>
       </c>
       <c r="B168">
-        <v>7.1661240000000003E-3</v>
+        <v>94.24</v>
       </c>
       <c r="C168">
         <v>17320.920999999998</v>
@@ -21748,7 +21745,7 @@
         <v>3.47</v>
       </c>
       <c r="R168">
-        <v>2.1030282120013677E-2</v>
+        <v>1923.57</v>
       </c>
     </row>
     <row r="169" spans="1:18" x14ac:dyDescent="0.35">
@@ -21756,7 +21753,7 @@
         <v>41820</v>
       </c>
       <c r="B169">
-        <v>-3.5197988999999999E-2</v>
+        <v>96.88</v>
       </c>
       <c r="C169">
         <v>17320.920999999998</v>
@@ -21804,7 +21801,7 @@
         <v>3.65</v>
       </c>
       <c r="R169">
-        <v>1.9058313448431896E-2</v>
+        <v>1960.23</v>
       </c>
     </row>
     <row r="170" spans="1:18" x14ac:dyDescent="0.35">
@@ -21812,7 +21809,7 @@
         <v>41851</v>
       </c>
       <c r="B170">
-        <v>7.5830756999999999E-2</v>
+        <v>97.85</v>
       </c>
       <c r="C170">
         <v>17622.257000000001</v>
@@ -21860,7 +21857,7 @@
         <v>3.97</v>
       </c>
       <c r="R170">
-        <v>-1.5079863077291922E-2</v>
+        <v>1930.67</v>
       </c>
     </row>
     <row r="171" spans="1:18" x14ac:dyDescent="0.35">
@@ -21868,7 +21865,7 @@
         <v>41882</v>
       </c>
       <c r="B171">
-        <v>-4.9752156999999998E-2</v>
+        <v>102</v>
       </c>
       <c r="C171">
         <v>17622.257000000001</v>
@@ -21916,7 +21913,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="R171">
-        <v>3.7655321727690261E-2</v>
+        <v>2003.37</v>
       </c>
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.35">
@@ -21924,7 +21921,7 @@
         <v>41912</v>
       </c>
       <c r="B172">
-        <v>3.4862733999999999E-2</v>
+        <v>100.76</v>
       </c>
       <c r="C172">
         <v>17622.257000000001</v>
@@ -21972,7 +21969,7 @@
         <v>4.51</v>
       </c>
       <c r="R172">
-        <v>-1.5513859147336717E-2</v>
+        <v>1972.29</v>
       </c>
     </row>
     <row r="173" spans="1:18" x14ac:dyDescent="0.35">
@@ -21980,7 +21977,7 @@
         <v>41943</v>
       </c>
       <c r="B173">
-        <v>-7.7711582000000001E-2</v>
+        <v>101.63</v>
       </c>
       <c r="C173">
         <v>17735.933000000001</v>
@@ -22028,7 +22025,7 @@
         <v>4.46</v>
       </c>
       <c r="R173">
-        <v>2.3201456175308888E-2</v>
+        <v>2018.05</v>
       </c>
     </row>
     <row r="174" spans="1:18" x14ac:dyDescent="0.35">
@@ -22036,7 +22033,7 @@
         <v>41973</v>
       </c>
       <c r="B174">
-        <v>-9.9748460000000008E-3</v>
+        <v>106.83</v>
       </c>
       <c r="C174">
         <v>17735.933000000001</v>
@@ -22084,7 +22081,7 @@
         <v>5.08</v>
       </c>
       <c r="R174">
-        <v>2.4533584400783015E-2</v>
+        <v>2067.56</v>
       </c>
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.35">
@@ -22092,7 +22089,7 @@
         <v>42004</v>
       </c>
       <c r="B175">
-        <v>-2.5196584000000001E-2</v>
+        <v>104.4</v>
       </c>
       <c r="C175">
         <v>17735.933000000001</v>
@@ -22140,7 +22137,7 @@
         <v>5.29</v>
       </c>
       <c r="R175">
-        <v>-4.1885120625277938E-3</v>
+        <v>2058.9</v>
       </c>
     </row>
     <row r="176" spans="1:18" x14ac:dyDescent="0.35">
@@ -22148,7 +22145,7 @@
         <v>42035</v>
       </c>
       <c r="B176">
-        <v>-2.1429752999999999E-2</v>
+        <v>100.36</v>
       </c>
       <c r="C176">
         <v>17874.715</v>
@@ -22196,7 +22193,7 @@
         <v>4.71</v>
       </c>
       <c r="R176">
-        <v>-3.1040847054252363E-2</v>
+        <v>1994.99</v>
       </c>
     </row>
     <row r="177" spans="1:18" x14ac:dyDescent="0.35">
@@ -22204,7 +22201,7 @@
         <v>42063</v>
       </c>
       <c r="B177">
-        <v>6.3814805000000002E-2</v>
+        <v>108.77</v>
       </c>
       <c r="C177">
         <v>17874.715</v>
@@ -22252,7 +22249,7 @@
         <v>4.66</v>
       </c>
       <c r="R177">
-        <v>5.4892505726845675E-2</v>
+        <v>2104.5</v>
       </c>
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.35">
@@ -22260,7 +22257,7 @@
         <v>42094</v>
       </c>
       <c r="B178">
-        <v>1.6553328999999999E-2</v>
+        <v>104.96</v>
       </c>
       <c r="C178">
         <v>17874.715</v>
@@ -22308,7 +22305,7 @@
         <v>4.63</v>
       </c>
       <c r="R178">
-        <v>-1.7396056070325572E-2</v>
+        <v>2067.89</v>
       </c>
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.35">
@@ -22316,7 +22313,7 @@
         <v>42124</v>
       </c>
       <c r="B179">
-        <v>6.3028989999999998E-3</v>
+        <v>107.27</v>
       </c>
       <c r="C179">
         <v>18093.223999999998</v>
@@ -22364,7 +22361,7 @@
         <v>4.51</v>
       </c>
       <c r="R179">
-        <v>8.5207627098153882E-3</v>
+        <v>2085.5100000000002</v>
       </c>
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.35">
@@ -22372,7 +22369,7 @@
         <v>42155</v>
       </c>
       <c r="B180">
-        <v>-3.9461879999999998E-3</v>
+        <v>109.78</v>
       </c>
       <c r="C180">
         <v>18093.223999999998</v>
@@ -22420,7 +22417,7 @@
         <v>4.66</v>
       </c>
       <c r="R180">
-        <v>1.0491438545008114E-2</v>
+        <v>2107.39</v>
       </c>
     </row>
     <row r="181" spans="1:18" x14ac:dyDescent="0.35">
@@ -22428,7 +22425,7 @@
         <v>42185</v>
       </c>
       <c r="B181">
-        <v>7.5631873000000002E-2</v>
+        <v>104.67</v>
       </c>
       <c r="C181">
         <v>18093.223999999998</v>
@@ -22476,7 +22473,7 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="R181">
-        <v>-2.10117728564716E-2</v>
+        <v>2063.11</v>
       </c>
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.35">
@@ -22484,7 +22481,7 @@
         <v>42216</v>
       </c>
       <c r="B182">
-        <v>-5.4283367999999999E-2</v>
+        <v>106.91</v>
       </c>
       <c r="C182">
         <v>18227.688999999998</v>
@@ -22532,7 +22529,7 @@
         <v>5.66</v>
       </c>
       <c r="R182">
-        <v>1.9742039930008559E-2</v>
+        <v>2103.84</v>
       </c>
     </row>
     <row r="183" spans="1:18" x14ac:dyDescent="0.35">
@@ -22540,7 +22537,7 @@
         <v>42247</v>
       </c>
       <c r="B183">
-        <v>3.6599206000000002E-2</v>
+        <v>100.64</v>
       </c>
       <c r="C183">
         <v>18227.688999999998</v>
@@ -22588,7 +22585,7 @@
         <v>5.87</v>
       </c>
       <c r="R183">
-        <v>-6.258080462392579E-2</v>
+        <v>1972.18</v>
       </c>
     </row>
     <row r="184" spans="1:18" x14ac:dyDescent="0.35">
@@ -22596,7 +22593,7 @@
         <v>42277</v>
       </c>
       <c r="B184">
-        <v>-1.9927704000000001E-2</v>
+        <v>98.9</v>
       </c>
       <c r="C184">
         <v>18227.688999999998</v>
@@ -22644,7 +22641,7 @@
         <v>6.2</v>
       </c>
       <c r="R184">
-        <v>-2.6442819620927094E-2</v>
+        <v>1920.03</v>
       </c>
     </row>
     <row r="185" spans="1:18" x14ac:dyDescent="0.35">
@@ -22652,7 +22649,7 @@
         <v>42308</v>
       </c>
       <c r="B185">
-        <v>-1.6858028000000001E-2</v>
+        <v>109.24</v>
       </c>
       <c r="C185">
         <v>18287.225999999999</v>
@@ -22700,7 +22697,7 @@
         <v>6.14</v>
       </c>
       <c r="R185">
-        <v>8.2983078389400333E-2</v>
+        <v>2079.36</v>
       </c>
     </row>
     <row r="186" spans="1:18" x14ac:dyDescent="0.35">
@@ -22708,7 +22705,7 @@
         <v>42338</v>
       </c>
       <c r="B186">
-        <v>2.0172911000000002E-2</v>
+        <v>110.3</v>
       </c>
       <c r="C186">
         <v>18287.225999999999</v>
@@ -22756,7 +22753,7 @@
         <v>6.87</v>
       </c>
       <c r="R186">
-        <v>5.0496306555847248E-4</v>
+        <v>2080.41</v>
       </c>
     </row>
     <row r="187" spans="1:18" x14ac:dyDescent="0.35">
@@ -22764,7 +22761,7 @@
         <v>42369</v>
       </c>
       <c r="B187">
-        <v>-3.243143E-3</v>
+        <v>107.03</v>
       </c>
       <c r="C187">
         <v>18287.225999999999</v>
@@ -22812,7 +22809,7 @@
         <v>7.63</v>
       </c>
       <c r="R187">
-        <v>-1.7530198374358763E-2</v>
+        <v>2043.94</v>
       </c>
     </row>
     <row r="188" spans="1:18" x14ac:dyDescent="0.35">
@@ -22820,7 +22817,7 @@
         <v>42400</v>
       </c>
       <c r="B188">
-        <v>-4.6474641999999997E-2</v>
+        <v>101.01</v>
       </c>
       <c r="C188">
         <v>18325.187000000002</v>
@@ -22868,7 +22865,7 @@
         <v>8.23</v>
       </c>
       <c r="R188">
-        <v>-5.0735344481736222E-2</v>
+        <v>1940.24</v>
       </c>
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.35">
@@ -22876,7 +22873,7 @@
         <v>42429</v>
       </c>
       <c r="B189">
-        <v>-1.7193469999999999E-2</v>
+        <v>99.74</v>
       </c>
       <c r="C189">
         <v>18325.187000000002</v>
@@ -22924,7 +22921,7 @@
         <v>6.98</v>
       </c>
       <c r="R189">
-        <v>-4.1283552550199776E-3</v>
+        <v>1932.23</v>
       </c>
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.35">
@@ -22932,7 +22929,7 @@
         <v>42460</v>
       </c>
       <c r="B190">
-        <v>-6.8887451000000002E-2</v>
+        <v>108.5</v>
       </c>
       <c r="C190">
         <v>18325.187000000002</v>
@@ -22980,7 +22977,7 @@
         <v>6.62</v>
       </c>
       <c r="R190">
-        <v>6.5991108718941094E-2</v>
+        <v>2059.7399999999998</v>
       </c>
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.35">
@@ -22988,7 +22985,7 @@
         <v>42490</v>
       </c>
       <c r="B191">
-        <v>2.1473406E-2</v>
+        <v>102.28</v>
       </c>
       <c r="C191">
         <v>18538.039000000001</v>
@@ -23036,7 +23033,7 @@
         <v>6.26</v>
       </c>
       <c r="R191">
-        <v>2.69936982337593E-3</v>
+        <v>2065.3000000000002</v>
       </c>
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.35">
@@ -23044,7 +23041,7 @@
         <v>42521</v>
       </c>
       <c r="B192">
-        <v>-1.5449667E-2</v>
+        <v>108.09</v>
       </c>
       <c r="C192">
         <v>18538.039000000001</v>
@@ -23092,7 +23089,7 @@
         <v>6.1</v>
       </c>
       <c r="R192">
-        <v>1.5329492083474561E-2</v>
+        <v>2096.96</v>
       </c>
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.35">
@@ -23100,7 +23097,7 @@
         <v>42551</v>
       </c>
       <c r="B193">
-        <v>-6.3152282000000004E-2</v>
+        <v>105.28</v>
       </c>
       <c r="C193">
         <v>18538.039000000001</v>
@@ -23148,7 +23145,7 @@
         <v>5.65</v>
       </c>
       <c r="R193">
-        <v>9.0607355409733081E-4</v>
+        <v>2098.86</v>
       </c>
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.35">
@@ -23156,7 +23153,7 @@
         <v>42582</v>
       </c>
       <c r="B194">
-        <v>9.6915620000000008E-3</v>
+        <v>114.13</v>
       </c>
       <c r="C194">
         <v>18729.13</v>
@@ -23204,7 +23201,7 @@
         <v>5.3</v>
       </c>
       <c r="R194">
-        <v>3.5609807228685897E-2</v>
+        <v>2173.6</v>
       </c>
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.35">
@@ -23212,7 +23209,7 @@
         <v>42613</v>
       </c>
       <c r="B195">
-        <v>5.8799576999999999E-2</v>
+        <v>116.57</v>
       </c>
       <c r="C195">
         <v>18729.13</v>
@@ -23260,7 +23257,7 @@
         <v>5.15</v>
       </c>
       <c r="R195">
-        <v>-1.2191755612808164E-3</v>
+        <v>2170.9499999999998</v>
       </c>
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.35">
@@ -23268,7 +23265,7 @@
         <v>42643</v>
       </c>
       <c r="B196">
-        <v>1.7948930000000001E-3</v>
+        <v>119</v>
       </c>
       <c r="C196">
         <v>18729.13</v>
@@ -23316,7 +23313,7 @@
         <v>4.74</v>
       </c>
       <c r="R196">
-        <v>-1.2344825997834263E-3</v>
+        <v>2168.27</v>
       </c>
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.35">
@@ -23324,7 +23321,7 @@
         <v>42674</v>
       </c>
       <c r="B197">
-        <v>-8.0925790000000008E-3</v>
+        <v>118.59</v>
       </c>
       <c r="C197">
         <v>18905.544999999998</v>
@@ -23372,7 +23369,7 @@
         <v>4.8899999999999997</v>
       </c>
       <c r="R197">
-        <v>-1.9425625037472249E-2</v>
+        <v>2126.15</v>
       </c>
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.35">
@@ -23380,7 +23377,7 @@
         <v>42704</v>
       </c>
       <c r="B198">
-        <v>5.2107279999999999E-2</v>
+        <v>118.94</v>
       </c>
       <c r="C198">
         <v>18905.544999999998</v>
@@ -23428,7 +23425,7 @@
         <v>4.28</v>
       </c>
       <c r="R198">
-        <v>3.4174446769983158E-2</v>
+        <v>2198.81</v>
       </c>
     </row>
     <row r="199" spans="1:18" x14ac:dyDescent="0.35">
@@ -23436,7 +23433,7 @@
         <v>42735</v>
       </c>
       <c r="B199">
-        <v>-3.5951735999999998E-2</v>
+        <v>120.25</v>
       </c>
       <c r="C199">
         <v>18905.544999999998</v>
@@ -23484,7 +23481,7 @@
         <v>4.01</v>
       </c>
       <c r="R199">
-        <v>1.8200754044233047E-2</v>
+        <v>2238.83</v>
       </c>
     </row>
     <row r="200" spans="1:18" x14ac:dyDescent="0.35">
@@ -23492,7 +23489,7 @@
         <v>42766</v>
       </c>
       <c r="B200">
-        <v>-1.2482775E-2</v>
+        <v>125.92</v>
       </c>
       <c r="C200">
         <v>19057.705000000002</v>
@@ -23540,7 +23537,7 @@
         <v>3.85</v>
       </c>
       <c r="R200">
-        <v>1.7884341374735824E-2</v>
+        <v>2278.87</v>
       </c>
     </row>
     <row r="201" spans="1:18" x14ac:dyDescent="0.35">
@@ -23548,7 +23545,7 @@
         <v>42794</v>
       </c>
       <c r="B201">
-        <v>-4.6967940999999999E-2</v>
+        <v>132.15</v>
       </c>
       <c r="C201">
         <v>19057.705000000002</v>
@@ -23596,7 +23593,7 @@
         <v>3.9</v>
       </c>
       <c r="R201">
-        <v>3.7198260541408734E-2</v>
+        <v>2363.64</v>
       </c>
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.35">
@@ -23604,7 +23601,7 @@
         <v>42825</v>
       </c>
       <c r="B202">
-        <v>8.0205580000000005E-3</v>
+        <v>135.16999999999999</v>
       </c>
       <c r="C202">
         <v>19057.705000000002</v>
@@ -23652,7 +23649,7 @@
         <v>3.91</v>
       </c>
       <c r="R202">
-        <v>-3.8923017041514463E-4</v>
+        <v>2362.7199999999998</v>
       </c>
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.35">
@@ -23660,7 +23657,7 @@
         <v>42855</v>
       </c>
       <c r="B203">
-        <v>-6.4985299999999998E-3</v>
+        <v>138.21</v>
       </c>
       <c r="C203">
         <v>19250.008999999998</v>
@@ -23708,7 +23705,7 @@
         <v>3.74</v>
       </c>
       <c r="R203">
-        <v>9.0912169025529899E-3</v>
+        <v>2384.1999999999998</v>
       </c>
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.35">
@@ -23716,7 +23713,7 @@
         <v>42886</v>
       </c>
       <c r="B204">
-        <v>-3.9316239000000003E-2</v>
+        <v>144.19999999999999</v>
       </c>
       <c r="C204">
         <v>19250.008999999998</v>
@@ -23764,7 +23761,7 @@
         <v>3.75</v>
       </c>
       <c r="R204">
-        <v>1.1576210049492719E-2</v>
+        <v>2411.8000000000002</v>
       </c>
     </row>
     <row r="205" spans="1:18" x14ac:dyDescent="0.35">
@@ -23772,7 +23769,7 @@
         <v>42916</v>
       </c>
       <c r="B205">
-        <v>3.4761209000000001E-2</v>
+        <v>139.72</v>
       </c>
       <c r="C205">
         <v>19250.008999999998</v>
@@ -23820,7 +23817,7 @@
         <v>3.69</v>
       </c>
       <c r="R205">
-        <v>4.8138319927024664E-3</v>
+        <v>2423.41</v>
       </c>
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.35">
@@ -23828,7 +23825,7 @@
         <v>42947</v>
       </c>
       <c r="B206">
-        <v>-2.5043112999999999E-2</v>
+        <v>144.81</v>
       </c>
       <c r="C206">
         <v>19495.475999999999</v>
@@ -23876,7 +23873,7 @@
         <v>3.83</v>
       </c>
       <c r="R206">
-        <v>1.9348768883515444E-2</v>
+        <v>2470.3000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -23888,7 +23885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="P2" sqref="B1:P2"/>
     </sheetView>
   </sheetViews>

</xml_diff>